<commit_message>
Envois de mail lors du register
</commit_message>
<xml_diff>
--- a/docs/PlanificationV2.xlsx
+++ b/docs/PlanificationV2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\var\www\Flavio_Soares_Rodrigues_TPI_2023\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\var\www\Flavio_Soares_Rodrigues_TPI_2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CFF079-41C7-4772-A350-57F75254E85C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90427709-B692-472C-8273-4344B94E4162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning réel" sheetId="4" r:id="rId1"/>
@@ -77,143 +77,143 @@
     <t>Totaux</t>
   </si>
   <si>
+    <t>Lecture de l'énoncé</t>
+  </si>
+  <si>
+    <t>Données utilisé pour la mise en forme conditionnelle</t>
+  </si>
+  <si>
+    <t>Tests et débogage</t>
+  </si>
+  <si>
+    <t>Documentation technique</t>
+  </si>
+  <si>
+    <t>Journal de bord</t>
+  </si>
+  <si>
+    <t>Documentation utilisateur</t>
+  </si>
+  <si>
+    <t>Rapport TPI</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Démarrage du projet</t>
+  </si>
+  <si>
+    <t>Réalisation du modèle conceptuel de données</t>
+  </si>
+  <si>
+    <t>Plannification</t>
+  </si>
+  <si>
+    <t>Réalisation du planning prévisionnel</t>
+  </si>
+  <si>
+    <t>Réalisation des maquettes d'interface utilisateur</t>
+  </si>
+  <si>
+    <t>Page d'accueil</t>
+  </si>
+  <si>
+    <t>Réalisation du backlog</t>
+  </si>
+  <si>
+    <t>Page d'inscription</t>
+  </si>
+  <si>
+    <t>Page de connexion</t>
+  </si>
+  <si>
+    <t>Barre de navigation</t>
+  </si>
+  <si>
+    <t>Page validation commande</t>
+  </si>
+  <si>
+    <t>Page ajouter un nouvel article (admin)</t>
+  </si>
+  <si>
+    <t>Implémentation</t>
+  </si>
+  <si>
+    <t>Test et débogage</t>
+  </si>
+  <si>
+    <t>Démarrage du projet + plannification</t>
+  </si>
+  <si>
+    <t>Visualisation de la répartition du temps de travail</t>
+  </si>
+  <si>
+    <t>Temps disponible sur 11j de travail en heures</t>
+  </si>
+  <si>
+    <t>Temps pour 1j de travail en heures</t>
+  </si>
+  <si>
+    <t>Page détails d'un article</t>
+  </si>
+  <si>
+    <t>Réalisation des tests et débogage</t>
+  </si>
+  <si>
+    <t>Page de déconnexion</t>
+  </si>
+  <si>
+    <t>Page de recherche (lors d'un filtre)</t>
+  </si>
+  <si>
+    <t>Page panier</t>
+  </si>
+  <si>
+    <t>Page ajouter une nouvelle catégorie (admin)</t>
+  </si>
+  <si>
+    <t>Page modifier un article (admin)</t>
+  </si>
+  <si>
+    <t>Page modifier une catégorie (admin)</t>
+  </si>
+  <si>
+    <t>Frontend (vues JS/HTML/CSS)</t>
+  </si>
+  <si>
+    <t>Fonctions de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Fonctions des articles</t>
+  </si>
+  <si>
+    <t>Fonctions des categories</t>
+  </si>
+  <si>
+    <t>Fonctions des images</t>
+  </si>
+  <si>
+    <t>Fonctions des villes</t>
+  </si>
+  <si>
+    <t>Fonctions des objets dans le panier</t>
+  </si>
+  <si>
+    <t>Backend (fonctions PHP liée à la base de données)</t>
+  </si>
+  <si>
+    <t>Base de données</t>
+  </si>
+  <si>
+    <t>Mise en place de la base de données</t>
+  </si>
+  <si>
     <t>Temps
-nécessaire</t>
-  </si>
-  <si>
-    <t>Lecture de l'énoncé</t>
-  </si>
-  <si>
-    <t>Temps total (tâches)</t>
-  </si>
-  <si>
-    <t>Données utilisé pour la mise en forme conditionnelle</t>
-  </si>
-  <si>
-    <t>Tests et débogage</t>
-  </si>
-  <si>
-    <t>Documentation technique</t>
-  </si>
-  <si>
-    <t>Journal de bord</t>
-  </si>
-  <si>
-    <t>Documentation utilisateur</t>
-  </si>
-  <si>
-    <t>Rapport TPI</t>
-  </si>
-  <si>
-    <t>Documentation</t>
-  </si>
-  <si>
-    <t>Démarrage du projet</t>
-  </si>
-  <si>
-    <t>Réalisation du modèle conceptuel de données</t>
-  </si>
-  <si>
-    <t>Plannification</t>
-  </si>
-  <si>
-    <t>Réalisation du planning prévisionnel</t>
-  </si>
-  <si>
-    <t>Réalisation des maquettes d'interface utilisateur</t>
-  </si>
-  <si>
-    <t>Page d'accueil</t>
-  </si>
-  <si>
-    <t>Réalisation du backlog</t>
-  </si>
-  <si>
-    <t>Page d'inscription</t>
-  </si>
-  <si>
-    <t>Page de connexion</t>
-  </si>
-  <si>
-    <t>Barre de navigation</t>
-  </si>
-  <si>
-    <t>Page validation commande</t>
-  </si>
-  <si>
-    <t>Page ajouter un nouvel article (admin)</t>
-  </si>
-  <si>
-    <t>Implémentation</t>
-  </si>
-  <si>
-    <t>Test et débogage</t>
-  </si>
-  <si>
-    <t>Démarrage du projet + plannification</t>
-  </si>
-  <si>
-    <t>Visualisation de la répartition du temps de travail</t>
-  </si>
-  <si>
-    <t>Temps disponible sur 11j de travail en heures</t>
-  </si>
-  <si>
-    <t>Temps pour 1j de travail en heures</t>
-  </si>
-  <si>
-    <t>Page détails d'un article</t>
-  </si>
-  <si>
-    <t>Réalisation des tests et débogage</t>
-  </si>
-  <si>
-    <t>Page de déconnexion</t>
-  </si>
-  <si>
-    <t>Page de recherche (lors d'un filtre)</t>
-  </si>
-  <si>
-    <t>Page panier</t>
-  </si>
-  <si>
-    <t>Page ajouter une nouvelle catégorie (admin)</t>
-  </si>
-  <si>
-    <t>Page modifier un article (admin)</t>
-  </si>
-  <si>
-    <t>Page modifier une catégorie (admin)</t>
-  </si>
-  <si>
-    <t>Frontend (vues JS/HTML/CSS)</t>
-  </si>
-  <si>
-    <t>Fonctions de l'utilisateur</t>
-  </si>
-  <si>
-    <t>Fonctions des articles</t>
-  </si>
-  <si>
-    <t>Fonctions des categories</t>
-  </si>
-  <si>
-    <t>Fonctions des images</t>
-  </si>
-  <si>
-    <t>Fonctions des villes</t>
-  </si>
-  <si>
-    <t>Fonctions des objets dans le panier</t>
-  </si>
-  <si>
-    <t>Backend (fonctions PHP liée à la base de données)</t>
-  </si>
-  <si>
-    <t>Base de données</t>
-  </si>
-  <si>
-    <t>Mise en place de la base de données</t>
+prévisionnel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temps réel </t>
   </si>
 </sst>
 </file>
@@ -876,6 +876,12 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -901,12 +907,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1649,8 +1649,8 @@
   </sheetPr>
   <dimension ref="B1:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -1669,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>1</v>
@@ -1705,12 +1705,12 @@
         <v>11</v>
       </c>
       <c r="O2" s="13" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="30"/>
@@ -1728,7 +1728,7 @@
     </row>
     <row r="4" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="7">
         <v>4.1666666666666664E-2</v>
@@ -1753,7 +1753,7 @@
     </row>
     <row r="5" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="24"/>
@@ -1771,7 +1771,7 @@
     </row>
     <row r="6" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C6" s="7">
         <v>0.10416666666666667</v>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="7" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="7">
         <v>0.14583333333333334</v>
@@ -1827,7 +1827,7 @@
     </row>
     <row r="8" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" s="7">
         <v>6.25E-2</v>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="9" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="7">
         <v>8.3333333333333329E-2</v>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="10" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="24"/>
@@ -1895,7 +1895,7 @@
     </row>
     <row r="11" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" s="7">
         <v>8.3333333333333329E-2</v>
@@ -1920,7 +1920,7 @@
     </row>
     <row r="12" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="24"/>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="13" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" s="7">
         <v>0.125</v>
@@ -1965,7 +1965,7 @@
     </row>
     <row r="14" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C14" s="7">
         <v>0.14583333333333334</v>
@@ -1992,7 +1992,7 @@
     </row>
     <row r="15" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" s="7">
         <v>5.5555555555555552E-2</v>
@@ -2019,7 +2019,7 @@
     </row>
     <row r="16" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C16" s="7">
         <v>0.10416666666666667</v>
@@ -2046,7 +2046,7 @@
     </row>
     <row r="17" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C17" s="7">
         <v>2.0833333333333332E-2</v>
@@ -2073,7 +2073,7 @@
     </row>
     <row r="18" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18" s="7">
         <v>7.6388888888888895E-2</v>
@@ -2098,7 +2098,7 @@
     </row>
     <row r="19" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="24"/>
@@ -2116,7 +2116,7 @@
     </row>
     <row r="20" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C20" s="7">
         <v>8.3333333333333329E-2</v>
@@ -2143,7 +2143,7 @@
     </row>
     <row r="21" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C21" s="7">
         <v>3.472222222222222E-3</v>
@@ -2168,7 +2168,7 @@
     </row>
     <row r="22" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C22" s="7">
         <v>0.14583333333333334</v>
@@ -2182,7 +2182,7 @@
         <v>0.21180555555555555</v>
       </c>
       <c r="J22" s="4">
-        <v>2.0833333333333332E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
@@ -2190,12 +2190,12 @@
       <c r="N22" s="23"/>
       <c r="O22" s="9">
         <f t="shared" si="2"/>
-        <v>0.2326388888888889</v>
+        <v>0.25347222222222221</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C23" s="7">
         <v>6.25E-2</v>
@@ -2218,7 +2218,7 @@
     </row>
     <row r="24" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C24" s="7">
         <v>0.10416666666666667</v>
@@ -2241,7 +2241,7 @@
     </row>
     <row r="25" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C25" s="7">
         <v>8.3333333333333329E-2</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="26" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C26" s="7">
         <v>0.10416666666666667</v>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="27" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C27" s="7">
         <v>0.10069444444444443</v>
@@ -2310,7 +2310,7 @@
     </row>
     <row r="28" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C28" s="7">
         <v>4.1666666666666664E-2</v>
@@ -2333,7 +2333,7 @@
     </row>
     <row r="29" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C29" s="7">
         <v>0.125</v>
@@ -2344,19 +2344,21 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
+      <c r="J29" s="4">
+        <v>0.125</v>
+      </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="23"/>
       <c r="O29" s="9">
         <f>SUM(D29:N29)</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="30" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C30" s="7">
         <v>2.7777777777777776E-2</v>
@@ -2379,7 +2381,7 @@
     </row>
     <row r="31" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C31" s="7">
         <v>0.125</v>
@@ -2402,7 +2404,7 @@
     </row>
     <row r="32" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C32" s="7">
         <v>2.7777777777777776E-2</v>
@@ -2425,7 +2427,7 @@
     </row>
     <row r="33" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C33" s="20"/>
       <c r="D33" s="24"/>
@@ -2443,7 +2445,7 @@
     </row>
     <row r="34" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C34" s="7">
         <v>0.22916666666666666</v>
@@ -2466,19 +2468,21 @@
       <c r="I34" s="4">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="J34" s="4"/>
+      <c r="J34" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="23"/>
       <c r="O34" s="9">
         <f t="shared" si="0"/>
-        <v>0.13541666666666666</v>
+        <v>0.15625</v>
       </c>
     </row>
     <row r="35" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C35" s="7">
         <v>0.20833333333333334</v>
@@ -2501,7 +2505,7 @@
     </row>
     <row r="36" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C36" s="7">
         <v>0.75</v>
@@ -2530,7 +2534,7 @@
     </row>
     <row r="37" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C37" s="7">
         <v>6.25E-2</v>
@@ -2553,7 +2557,7 @@
     </row>
     <row r="38" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C38" s="20"/>
       <c r="D38" s="24"/>
@@ -2571,7 +2575,7 @@
     </row>
     <row r="39" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C39" s="8">
         <v>0.33333333333333331</v>
@@ -2589,7 +2593,7 @@
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="J39" s="28">
-        <v>6.25E-2</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="K39" s="28"/>
       <c r="L39" s="28"/>
@@ -2597,7 +2601,7 @@
       <c r="N39" s="29"/>
       <c r="O39" s="9">
         <f t="shared" si="0"/>
-        <v>0.21527777777777779</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="40" spans="2:16" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2633,8 +2637,8 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="J40" s="5">
-        <f t="shared" si="3"/>
-        <v>8.3333333333333329E-2</v>
+        <f>SUM(J3:J39)</f>
+        <v>0.33333333333333337</v>
       </c>
       <c r="K40" s="5">
         <f t="shared" si="3"/>
@@ -2654,7 +2658,7 @@
       </c>
       <c r="O40" s="6">
         <f>SUM(D40:N40)</f>
-        <v>2.083333333333333</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="P40" s="4"/>
     </row>
@@ -2704,17 +2708,17 @@
       <c r="O43" s="4"/>
     </row>
     <row r="44" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="C44" s="41"/>
+      <c r="B44" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="43"/>
       <c r="D44" s="4"/>
-      <c r="E44" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="F44" s="43"/>
-      <c r="G44" s="43"/>
-      <c r="H44" s="44"/>
+      <c r="E44" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="F44" s="45"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="46"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
@@ -2725,17 +2729,17 @@
     </row>
     <row r="45" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C45" s="37">
         <v>3.6666666666666665</v>
       </c>
       <c r="D45" s="4"/>
-      <c r="E45" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="F45" s="46"/>
-      <c r="G45" s="46"/>
+      <c r="E45" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="F45" s="48"/>
+      <c r="G45" s="48"/>
       <c r="H45" s="37">
         <f>SUM(C4:C4,C6:C9)</f>
         <v>0.4375</v>
@@ -2750,17 +2754,17 @@
     </row>
     <row r="46" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="36" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C46" s="39">
         <v>0.33333333333333331</v>
       </c>
       <c r="D46" s="4"/>
-      <c r="E46" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="F46" s="48"/>
-      <c r="G46" s="48"/>
+      <c r="E46" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="F46" s="50"/>
+      <c r="G46" s="50"/>
       <c r="H46" s="38">
         <f>SUM(C13:C15,C16:C18,C32,C28,C19:C22,C23:C24,C25,C26,C27,C29,C30,C31)</f>
         <v>1.5625</v>
@@ -2774,22 +2778,22 @@
       <c r="O46" s="4"/>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E47" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="F47" s="48"/>
-      <c r="G47" s="48"/>
+      <c r="E47" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
       <c r="H47" s="38">
         <f>SUM(C34:C37)</f>
         <v>1.25</v>
       </c>
     </row>
     <row r="48" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E48" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="F48" s="50"/>
-      <c r="G48" s="50"/>
+      <c r="E48" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48" s="41"/>
+      <c r="G48" s="41"/>
       <c r="H48" s="39">
         <f>SUM(C39:C39)</f>
         <v>0.33333333333333331</v>

</xml_diff>

<commit_message>
Mise à jour de la doc technique
</commit_message>
<xml_diff>
--- a/docs/PlanificationV2.xlsx
+++ b/docs/PlanificationV2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\var\www\Flavio_Soares_Rodrigues_TPI_2023\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\var\www\Flavio_Soares_Rodrigues_TPI_2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C62236-B78D-469E-BC99-B7EA9B7D8224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBD075F-4D56-4583-B4EB-B09BE24ED301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3870" windowWidth="28800" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="33315" yWindow="7950" windowWidth="18900" windowHeight="12795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning réel" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>Page d'accueil</t>
-  </si>
-  <si>
-    <t>Réalisation du backlog</t>
   </si>
   <si>
     <t>Page d'inscription</t>
@@ -266,7 +263,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,20 +288,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="38">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -608,21 +593,6 @@
       <top/>
       <bottom style="thin">
         <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -769,7 +739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -870,46 +840,46 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -918,30 +888,14 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="44">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -1665,10 +1619,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:P48"/>
+  <dimension ref="B1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -1687,7 +1641,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>1</v>
@@ -1723,7 +1677,7 @@
         <v>11</v>
       </c>
       <c r="O2" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -1765,7 +1719,7 @@
       <c r="M4" s="4"/>
       <c r="N4" s="23"/>
       <c r="O4" s="9">
-        <f t="shared" ref="O4:O39" si="0">SUM(D4:N4)</f>
+        <f t="shared" ref="O4:O38" si="0">SUM(D4:N4)</f>
         <v>3.4722222222222224E-2</v>
       </c>
     </row>
@@ -1843,7 +1797,7 @@
         <v>0.17013888888888887</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1870,115 +1824,119 @@
         <v>5.5555555555555559E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="7">
+    <row r="9" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="21"/>
+    </row>
+    <row r="10" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="34">
-        <f>SUM(D9:N9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="21"/>
-    </row>
-    <row r="11" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="7">
+      <c r="D10" s="22"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4">
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="9">
+        <f t="shared" ref="O10" si="1">SUM(D10:N10)</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="9">
-        <f t="shared" ref="O11" si="1">SUM(D11:N11)</f>
+    </row>
+    <row r="11" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="21"/>
+    </row>
+    <row r="12" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="D12" s="22"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G12" s="4">
         <v>8.3333333333333329E-2</v>
       </c>
-    </row>
-    <row r="12" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="21"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="9">
+        <f t="shared" si="0"/>
+        <v>9.722222222222221E-2</v>
+      </c>
     </row>
     <row r="13" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C13" s="7">
-        <v>0.125</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="G13" s="4">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="23"/>
-      <c r="O13" s="9">
-        <f t="shared" si="0"/>
-        <v>9.722222222222221E-2</v>
+      <c r="O13" s="33">
+        <f>SUM(D13:N13)</f>
+        <v>0.18055555555555555</v>
       </c>
     </row>
     <row r="14" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1986,17 +1944,17 @@
         <v>49</v>
       </c>
       <c r="C14" s="7">
-        <v>0.14583333333333334</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4">
-        <v>0.16666666666666666</v>
-      </c>
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="G14" s="4">
+        <v>6.25E-2</v>
+      </c>
+      <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -2005,7 +1963,7 @@
       <c r="N14" s="23"/>
       <c r="O14" s="33">
         <f>SUM(D14:N14)</f>
-        <v>0.18055555555555555</v>
+        <v>7.2916666666666671E-2</v>
       </c>
     </row>
     <row r="15" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2013,7 +1971,7 @@
         <v>50</v>
       </c>
       <c r="C15" s="7">
-        <v>5.5555555555555552E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="4"/>
@@ -2021,7 +1979,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="G15" s="4">
-        <v>6.25E-2</v>
+        <v>6.9444444444444434E-2</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -2030,9 +1988,9 @@
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="23"/>
-      <c r="O15" s="33">
-        <f>SUM(D15:N15)</f>
-        <v>7.2916666666666671E-2</v>
+      <c r="O15" s="9">
+        <f t="shared" si="0"/>
+        <v>7.9861111111111105E-2</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2040,15 +1998,15 @@
         <v>51</v>
       </c>
       <c r="C16" s="7">
-        <v>0.10416666666666667</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4">
-        <v>1.0416666666666666E-2</v>
+        <v>3.472222222222222E-3</v>
       </c>
       <c r="G16" s="4">
-        <v>6.9444444444444434E-2</v>
+        <v>3.4722222222222224E-2</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -2058,165 +2016,165 @@
       <c r="M16" s="4"/>
       <c r="N16" s="23"/>
       <c r="O16" s="9">
-        <f t="shared" si="0"/>
-        <v>7.9861111111111105E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+        <f>SUM(D16:N16)</f>
+        <v>3.8194444444444448E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C17" s="7">
-        <v>2.0833333333333332E-2</v>
+        <v>7.6388888888888895E-2</v>
       </c>
       <c r="D17" s="22"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4">
-        <v>3.472222222222222E-3</v>
-      </c>
-      <c r="G17" s="4">
-        <v>3.4722222222222224E-2</v>
-      </c>
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
+      <c r="L17" s="4">
+        <v>2.4305555555555556E-2</v>
+      </c>
       <c r="M17" s="4"/>
       <c r="N17" s="23"/>
       <c r="O17" s="9">
         <f>SUM(D17:N17)</f>
-        <v>3.8194444444444448E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="7">
-        <v>7.6388888888888895E-2</v>
-      </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="9">
-        <f>SUM(D18:N18)</f>
-        <v>1.0416666666666666E-2</v>
-      </c>
+        <v>3.4722222222222224E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="20"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="21"/>
     </row>
     <row r="19" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="21"/>
+      <c r="B19" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I19" s="4">
+        <v>3.125E-2</v>
+      </c>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="9">
+        <f t="shared" ref="O19:O26" si="2">SUM(D19:N19)</f>
+        <v>0.11458333333333333</v>
+      </c>
     </row>
     <row r="20" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="52" t="s">
-        <v>29</v>
+      <c r="B20" s="50" t="s">
+        <v>40</v>
       </c>
       <c r="C20" s="7">
-        <v>8.3333333333333329E-2</v>
+        <v>3.472222222222222E-3</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="I20" s="4">
-        <v>3.125E-2</v>
-      </c>
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="23"/>
       <c r="O20" s="9">
-        <f t="shared" ref="O20:O27" si="2">SUM(D20:N20)</f>
-        <v>0.11458333333333333</v>
+        <f t="shared" si="2"/>
+        <v>3.472222222222222E-3</v>
       </c>
     </row>
     <row r="21" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="52" t="s">
-        <v>41</v>
+      <c r="B21" s="50" t="s">
+        <v>27</v>
       </c>
       <c r="C21" s="7">
-        <v>3.472222222222222E-3</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="4">
-        <v>3.472222222222222E-3</v>
-      </c>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4">
+        <v>0.21180555555555555</v>
+      </c>
+      <c r="J21" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="23"/>
       <c r="O21" s="9">
         <f t="shared" si="2"/>
-        <v>3.472222222222222E-3</v>
+        <v>0.25347222222222221</v>
       </c>
     </row>
     <row r="22" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="52" t="s">
-        <v>28</v>
+      <c r="B22" s="50" t="s">
+        <v>26</v>
       </c>
       <c r="C22" s="7">
-        <v>0.14583333333333334</v>
+        <v>6.25E-2</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
-      <c r="I22" s="4">
-        <v>0.21180555555555555</v>
-      </c>
-      <c r="J22" s="4">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="K22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4">
+        <v>6.25E-2</v>
+      </c>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
       <c r="N22" s="23"/>
       <c r="O22" s="9">
         <f t="shared" si="2"/>
-        <v>0.25347222222222221</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="52" t="s">
-        <v>26</v>
+      <c r="B23" s="50" t="s">
+        <v>29</v>
       </c>
       <c r="C23" s="7">
-        <v>6.25E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="4"/>
@@ -2226,22 +2184,22 @@
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4">
-        <v>6.25E-2</v>
+        <v>9.0277777777777776E-2</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="23"/>
-      <c r="O23" s="9">
+      <c r="O23" s="15">
         <f t="shared" si="2"/>
-        <v>6.25E-2</v>
+        <v>9.0277777777777776E-2</v>
       </c>
     </row>
     <row r="24" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="52" t="s">
-        <v>30</v>
+      <c r="B24" s="50" t="s">
+        <v>41</v>
       </c>
       <c r="C24" s="7">
-        <v>0.10416666666666667</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="4"/>
@@ -2251,22 +2209,22 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4">
-        <v>9.0277777777777776E-2</v>
+        <v>3.4722222222222224E-2</v>
       </c>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="23"/>
-      <c r="O24" s="15">
+      <c r="O24" s="9">
         <f t="shared" si="2"/>
-        <v>9.0277777777777776E-2</v>
+        <v>3.4722222222222224E-2</v>
       </c>
     </row>
     <row r="25" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="52" t="s">
-        <v>42</v>
+      <c r="B25" s="50" t="s">
+        <v>38</v>
       </c>
       <c r="C25" s="7">
-        <v>8.3333333333333329E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="4"/>
@@ -2276,22 +2234,22 @@
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4">
-        <v>3.4722222222222224E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="23"/>
       <c r="O25" s="9">
         <f t="shared" si="2"/>
-        <v>3.4722222222222224E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="26" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="52" t="s">
-        <v>39</v>
+      <c r="B26" s="50" t="s">
+        <v>42</v>
       </c>
       <c r="C26" s="7">
-        <v>0.10416666666666667</v>
+        <v>0.10069444444444443</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="4"/>
@@ -2300,23 +2258,22 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
-      <c r="K26" s="4">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="L26" s="4"/>
+      <c r="L26" s="4">
+        <v>0.15277777777777776</v>
+      </c>
       <c r="M26" s="4"/>
       <c r="N26" s="23"/>
       <c r="O26" s="9">
         <f t="shared" si="2"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.15277777777777776</v>
       </c>
     </row>
     <row r="27" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="51" t="s">
-        <v>43</v>
+      <c r="B27" s="50" t="s">
+        <v>30</v>
       </c>
       <c r="C27" s="7">
-        <v>0.10069444444444443</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="4"/>
@@ -2325,22 +2282,23 @@
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
       <c r="L27" s="4">
-        <v>8.3333333333333329E-2</v>
+        <v>5.2083333333333336E-2</v>
       </c>
       <c r="M27" s="4"/>
       <c r="N27" s="23"/>
       <c r="O27" s="9">
-        <f t="shared" si="2"/>
-        <v>8.3333333333333329E-2</v>
+        <f>SUM(D27:N27)</f>
+        <v>5.2083333333333336E-2</v>
       </c>
     </row>
     <row r="28" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="52" t="s">
+      <c r="B28" s="50" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="7">
-        <v>4.1666666666666664E-2</v>
+        <v>0.125</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="4"/>
@@ -2348,24 +2306,24 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
+      <c r="J28" s="4">
+        <v>0.125</v>
+      </c>
       <c r="K28" s="4"/>
-      <c r="L28" s="4">
-        <v>3.125E-2</v>
-      </c>
+      <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="23"/>
       <c r="O28" s="9">
         <f>SUM(D28:N28)</f>
-        <v>3.125E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="29" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="52" t="s">
-        <v>32</v>
+      <c r="B29" s="50" t="s">
+        <v>43</v>
       </c>
       <c r="C29" s="7">
-        <v>0.125</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="4"/>
@@ -2373,24 +2331,24 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
-      <c r="J29" s="4">
-        <v>0.125</v>
-      </c>
-      <c r="K29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="23"/>
       <c r="O29" s="9">
-        <f>SUM(D29:N29)</f>
+        <f t="shared" si="0"/>
+        <v>1.3888888888888888E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="7">
         <v>0.125</v>
-      </c>
-    </row>
-    <row r="30" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="7">
-        <v>2.7777777777777776E-2</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="4"/>
@@ -2399,23 +2357,23 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
-      <c r="K30" s="4">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="L30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="M30" s="4"/>
       <c r="N30" s="23"/>
-      <c r="O30" s="9">
+      <c r="O30" s="15">
         <f t="shared" si="0"/>
-        <v>1.3888888888888888E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="51" t="s">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="50" t="s">
         <v>45</v>
       </c>
       <c r="C31" s="7">
-        <v>0.125</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="4"/>
@@ -2424,109 +2382,115 @@
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4">
-        <v>4.1666666666666664E-2</v>
-      </c>
+      <c r="K31" s="4">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="L31" s="4"/>
       <c r="M31" s="4"/>
       <c r="N31" s="23"/>
-      <c r="O31" s="15">
+      <c r="O31" s="9">
+        <f>SUM(D31:N31)</f>
+        <v>1.3888888888888888E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="20"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="21"/>
+    </row>
+    <row r="33" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="7">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="D33" s="22">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="E33" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F33" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G33" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H33" s="4">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="I33" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J33" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="K33" s="4">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="L33" s="4">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="M33" s="4"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="9">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="52" t="s">
-        <v>46</v>
-      </c>
-      <c r="C32" s="7">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="D32" s="22"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="9">
-        <f>SUM(D32:N32)</f>
-        <v>1.3888888888888888E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="20"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="26"/>
-      <c r="O33" s="21"/>
+        <v>0.17708333333333334</v>
+      </c>
     </row>
     <row r="34" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C34" s="7">
-        <v>0.22916666666666666</v>
-      </c>
-      <c r="D34" s="22">
-        <v>3.4722222222222224E-2</v>
-      </c>
-      <c r="E34" s="4">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="F34" s="4">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G34" s="4">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="H34" s="4">
-        <v>1.7361111111111112E-2</v>
-      </c>
-      <c r="I34" s="4">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="J34" s="4">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="K34" s="4">
-        <v>1.3888888888888888E-2</v>
-      </c>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D34" s="22"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="23"/>
       <c r="O34" s="9">
         <f t="shared" si="0"/>
-        <v>0.1701388888888889</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C35" s="7">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="D35" s="22">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="E35" s="4">
+        <v>0.19791666666666666</v>
+      </c>
+      <c r="F35" s="4">
+        <v>0.15625</v>
+      </c>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
@@ -2537,25 +2501,19 @@
       <c r="N35" s="23"/>
       <c r="O35" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.38194444444444442</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C36" s="7">
-        <v>0.75</v>
-      </c>
-      <c r="D36" s="22">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="E36" s="4">
-        <v>0.19791666666666666</v>
-      </c>
-      <c r="F36" s="4">
-        <v>0.15625</v>
-      </c>
+        <v>6.25E-2</v>
+      </c>
+      <c r="D36" s="22"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
@@ -2564,144 +2522,138 @@
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
       <c r="N36" s="23"/>
-      <c r="O36" s="9">
-        <f t="shared" si="0"/>
-        <v>0.38194444444444442</v>
-      </c>
-    </row>
-    <row r="37" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" s="7">
-        <v>6.25E-2</v>
-      </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="23"/>
-      <c r="O37" s="15">
+      <c r="O36" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="19" t="s">
+    <row r="37" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
-      <c r="L38" s="25"/>
-      <c r="M38" s="25"/>
-      <c r="N38" s="26"/>
-      <c r="O38" s="21"/>
-    </row>
-    <row r="39" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="8">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D39" s="27"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28">
+      <c r="C37" s="20"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="25"/>
+      <c r="L37" s="25"/>
+      <c r="M37" s="25"/>
+      <c r="N37" s="26"/>
+      <c r="O37" s="21"/>
+    </row>
+    <row r="38" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="8">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D38" s="27"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28">
         <v>6.25E-2</v>
       </c>
-      <c r="H39" s="28">
+      <c r="H38" s="28">
         <v>6.25E-2</v>
       </c>
-      <c r="I39" s="28">
+      <c r="I38" s="28">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="J39" s="28">
+      <c r="J38" s="28">
         <v>0.14583333333333334</v>
       </c>
-      <c r="K39" s="28">
+      <c r="K38" s="28">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="L39" s="28"/>
-      <c r="M39" s="28"/>
-      <c r="N39" s="29"/>
-      <c r="O39" s="9">
+      <c r="L38" s="28">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="M38" s="28"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="9">
         <f t="shared" si="0"/>
-        <v>0.31944444444444448</v>
-      </c>
-    </row>
-    <row r="40" spans="2:16" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="14" t="s">
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="6">
-        <f t="shared" ref="C40:N40" si="3">SUM(C3:C39)</f>
+      <c r="C39" s="6">
+        <f t="shared" ref="C39:N39" si="3">SUM(C3:C38)</f>
         <v>3.6666666666666665</v>
       </c>
-      <c r="D40" s="5">
+      <c r="D39" s="5">
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E40" s="5">
+      <c r="E39" s="5">
         <f t="shared" si="3"/>
         <v>0.33333333333333337</v>
       </c>
-      <c r="F40" s="5">
+      <c r="F39" s="5">
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G39" s="5">
         <f t="shared" si="3"/>
         <v>0.33333333333333326</v>
       </c>
-      <c r="H40" s="5">
+      <c r="H39" s="5">
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="I40" s="5">
+      <c r="I39" s="5">
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="J40" s="5">
-        <f>SUM(J3:J39)</f>
+      <c r="J39" s="5">
+        <f>SUM(J3:J38)</f>
         <v>0.33333333333333337</v>
       </c>
-      <c r="K40" s="5">
+      <c r="K39" s="5">
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="L40" s="5">
+      <c r="L39" s="5">
         <f t="shared" si="3"/>
-        <v>0.15625</v>
-      </c>
-      <c r="M40" s="5">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M39" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N40" s="5">
+      <c r="N39" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O40" s="6">
-        <f>SUM(D40:N40)</f>
-        <v>2.8229166666666665</v>
-      </c>
-      <c r="P40" s="4"/>
-    </row>
-    <row r="41" spans="2:16" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O39" s="6">
+        <f>SUM(D39:N39)</f>
+        <v>3</v>
+      </c>
+      <c r="P39" s="4"/>
+    </row>
+    <row r="40" spans="2:16" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -2716,7 +2668,7 @@
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -2731,13 +2683,18 @@
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
     </row>
-    <row r="43" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="4"/>
+    <row r="43" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="42"/>
       <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
+      <c r="E43" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="45"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
@@ -2746,18 +2703,23 @@
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
     </row>
-    <row r="44" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="C44" s="43"/>
+    <row r="44" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="36">
+        <v>3.6666666666666665</v>
+      </c>
       <c r="D44" s="4"/>
-      <c r="E44" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="F44" s="45"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="46"/>
+      <c r="E44" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44" s="47"/>
+      <c r="G44" s="47"/>
+      <c r="H44" s="36">
+        <f>SUM(C4:C4,C6:C8)</f>
+        <v>0.35416666666666669</v>
+      </c>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
@@ -2766,22 +2728,22 @@
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
     </row>
-    <row r="45" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C45" s="37">
-        <v>3.6666666666666665</v>
+      <c r="C45" s="38">
+        <v>0.33333333333333331</v>
       </c>
       <c r="D45" s="4"/>
-      <c r="E45" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="F45" s="48"/>
-      <c r="G45" s="48"/>
+      <c r="E45" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="F45" s="49"/>
+      <c r="G45" s="49"/>
       <c r="H45" s="37">
-        <f>SUM(C4:C4,C6:C9)</f>
-        <v>0.4375</v>
+        <f>SUM(C12:C14,C15:C17,C31,C27,C18:C21,C22:C23,C24,C25,C26,C28,C29,C30)</f>
+        <v>1.5625</v>
       </c>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
@@ -2791,291 +2753,261 @@
       <c r="N45" s="4"/>
       <c r="O45" s="4"/>
     </row>
-    <row r="46" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="C46" s="39">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="49" t="s">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E46" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="49"/>
+      <c r="G46" s="49"/>
+      <c r="H46" s="37">
+        <f>SUM(C33:C36)</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E47" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="F46" s="50"/>
-      <c r="G46" s="50"/>
-      <c r="H46" s="38">
-        <f>SUM(C13:C15,C16:C18,C32,C28,C19:C22,C23:C24,C25,C26,C27,C29,C30,C31)</f>
-        <v>1.5625</v>
-      </c>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
-      <c r="O46" s="4"/>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E47" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="F47" s="50"/>
-      <c r="G47" s="50"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="40"/>
       <c r="H47" s="38">
-        <f>SUM(C34:C37)</f>
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="48" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E48" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="F48" s="41"/>
-      <c r="G48" s="41"/>
-      <c r="H48" s="39">
-        <f>SUM(C39:C39)</f>
-        <v>0.33333333333333331</v>
+        <f>SUM(C38:C38)</f>
+        <v>0.41666666666666669</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="E44:H44"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="E43:H43"/>
+    <mergeCell ref="E44:G44"/>
     <mergeCell ref="E45:G45"/>
     <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
   </mergeCells>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="44" priority="46">
-      <formula xml:space="preserve"> $C$40&lt;&gt;$C$45</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
-    <cfRule type="expression" dxfId="43" priority="45">
-      <formula xml:space="preserve"> $D$40&lt;&gt;$C$46</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28:N39 D27:J27 L27:N27 D3:N26">
-    <cfRule type="notContainsBlanks" dxfId="42" priority="47">
+  <conditionalFormatting sqref="C39">
+    <cfRule type="expression" dxfId="43" priority="46">
+      <formula xml:space="preserve"> $C$39&lt;&gt;$C$44</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="expression" dxfId="42" priority="45">
+      <formula xml:space="preserve"> $D$39&lt;&gt;$C$45</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:N38 D26:J26 L26:N26 D3:N25">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="47">
       <formula>LEN(TRIM(D3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
-    <cfRule type="expression" dxfId="41" priority="44">
-      <formula xml:space="preserve"> $E$40&lt;&gt;$C$46</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F40">
-    <cfRule type="expression" dxfId="40" priority="43">
-      <formula xml:space="preserve"> $F$40&lt;&gt;$C$46</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G40">
-    <cfRule type="expression" dxfId="39" priority="42">
-      <formula xml:space="preserve"> $G$40&lt;&gt;$C$46</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H40">
-    <cfRule type="expression" dxfId="38" priority="41">
-      <formula xml:space="preserve"> $H$40&lt;&gt;$C$46</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
-    <cfRule type="expression" dxfId="37" priority="40">
-      <formula xml:space="preserve"> $I$40&lt;&gt;$C$46</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J40">
-    <cfRule type="expression" dxfId="36" priority="39">
-      <formula xml:space="preserve"> $J$40&lt;&gt;$C$46</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K40">
-    <cfRule type="expression" dxfId="35" priority="38">
-      <formula xml:space="preserve"> $K$40&lt;&gt;$C$46</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L40">
-    <cfRule type="expression" dxfId="34" priority="37">
-      <formula xml:space="preserve"> $L$40&lt;&gt;$C$46</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M40">
-    <cfRule type="expression" dxfId="33" priority="36">
-      <formula xml:space="preserve"> $M$40&lt;&gt;$C$46</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N40">
-    <cfRule type="expression" dxfId="32" priority="35">
-      <formula xml:space="preserve"> $N$40&lt;&gt;$C$46</formula>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="expression" dxfId="40" priority="44">
+      <formula xml:space="preserve"> $E$39&lt;&gt;$C$45</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F39">
+    <cfRule type="expression" dxfId="39" priority="43">
+      <formula xml:space="preserve"> $F$39&lt;&gt;$C$45</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G39">
+    <cfRule type="expression" dxfId="38" priority="42">
+      <formula xml:space="preserve"> $G$39&lt;&gt;$C$45</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H39">
+    <cfRule type="expression" dxfId="37" priority="41">
+      <formula xml:space="preserve"> $H$39&lt;&gt;$C$45</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I39">
+    <cfRule type="expression" dxfId="36" priority="40">
+      <formula xml:space="preserve"> $I$39&lt;&gt;$C$45</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J39">
+    <cfRule type="expression" dxfId="35" priority="39">
+      <formula xml:space="preserve"> $J$39&lt;&gt;$C$45</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K39">
+    <cfRule type="expression" dxfId="34" priority="38">
+      <formula xml:space="preserve"> $K$39&lt;&gt;$C$45</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L39">
+    <cfRule type="expression" dxfId="33" priority="37">
+      <formula xml:space="preserve"> $L$39&lt;&gt;$C$45</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M39">
+    <cfRule type="expression" dxfId="32" priority="36">
+      <formula xml:space="preserve"> $M$39&lt;&gt;$C$45</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N39">
+    <cfRule type="expression" dxfId="31" priority="35">
+      <formula xml:space="preserve"> $N$39&lt;&gt;$C$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="expression" dxfId="31" priority="28">
+    <cfRule type="expression" dxfId="30" priority="28">
       <formula>$O$4&lt;&gt;$C$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O6">
-    <cfRule type="expression" dxfId="30" priority="30">
+    <cfRule type="expression" dxfId="29" priority="30">
       <formula>$O$6&lt;&gt;$C$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7">
-    <cfRule type="expression" dxfId="29" priority="31">
+    <cfRule type="expression" dxfId="28" priority="31">
       <formula>$O$7&lt;&gt;$C$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O8">
-    <cfRule type="expression" dxfId="28" priority="32">
+    <cfRule type="expression" dxfId="27" priority="32">
       <formula>$O$8&lt;&gt;$C$8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O9">
-    <cfRule type="expression" dxfId="27" priority="23">
-      <formula>$O$9&lt;&gt;$C$9</formula>
+  <conditionalFormatting sqref="O12">
+    <cfRule type="expression" dxfId="26" priority="22">
+      <formula>$O$12&lt;&gt;$C$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O13">
-    <cfRule type="expression" dxfId="26" priority="22">
+    <cfRule type="expression" dxfId="25" priority="21">
       <formula>$O$13&lt;&gt;$C$13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O14">
-    <cfRule type="expression" dxfId="25" priority="21">
+    <cfRule type="expression" dxfId="24" priority="20">
       <formula>$O$14&lt;&gt;$C$14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O15">
-    <cfRule type="expression" dxfId="24" priority="20">
+    <cfRule type="expression" dxfId="23" priority="19">
       <formula>$O$15&lt;&gt;$C$15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O16">
-    <cfRule type="expression" dxfId="23" priority="19">
+    <cfRule type="expression" dxfId="22" priority="18">
       <formula>$O$16&lt;&gt;$C$16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O17">
-    <cfRule type="expression" dxfId="22" priority="18">
+    <cfRule type="expression" dxfId="21" priority="17">
       <formula>$O$17&lt;&gt;$C$17</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="O31">
+    <cfRule type="expression" dxfId="20" priority="16">
+      <formula>$O$31&lt;&gt;$C$31</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O27">
+    <cfRule type="expression" dxfId="19" priority="15">
+      <formula>$O$27&lt;&gt;$C$27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O19">
+    <cfRule type="expression" dxfId="18" priority="14">
+      <formula>$O$19&lt;&gt;$C$19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O20">
+    <cfRule type="expression" dxfId="17" priority="13">
+      <formula>$O$20&lt;&gt;$C$20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O21">
+    <cfRule type="expression" dxfId="16" priority="12">
+      <formula>$O$21&lt;&gt;$C$21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O22">
+    <cfRule type="expression" dxfId="15" priority="11">
+      <formula>$O$22&lt;&gt;$C$22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O23">
+    <cfRule type="expression" dxfId="14" priority="10">
+      <formula>$O$23&lt;&gt;$C$23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O24">
+    <cfRule type="expression" dxfId="13" priority="9">
+      <formula>$O$24&lt;&gt;$C$24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O25 O27">
+    <cfRule type="expression" dxfId="12" priority="8">
+      <formula>$O$25&lt;&gt;$C$25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O26:O27">
+    <cfRule type="expression" dxfId="11" priority="7">
+      <formula>$O$26&lt;&gt;$C$26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O28">
+    <cfRule type="expression" dxfId="10" priority="6">
+      <formula>$O$28&lt;&gt;$C$28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O29">
+    <cfRule type="expression" dxfId="9" priority="5">
+      <formula>$O$29&lt;&gt;$C$29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O30:O31">
+    <cfRule type="expression" dxfId="8" priority="4">
+      <formula>$O$30&lt;&gt;$C$30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O33">
+    <cfRule type="expression" dxfId="7" priority="27">
+      <formula>$O$33&lt;&gt;$C$33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O34">
+    <cfRule type="expression" dxfId="6" priority="26">
+      <formula>$O$34&lt;&gt;$C$34</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O35">
+    <cfRule type="expression" dxfId="5" priority="25">
+      <formula>$O$35&lt;&gt;$C$35</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O36">
+    <cfRule type="expression" dxfId="4" priority="24">
+      <formula>$O$36&lt;&gt;$C$36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O38">
+    <cfRule type="expression" dxfId="3" priority="33">
+      <formula xml:space="preserve"> $O$38&lt;&gt;$C$38</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O39">
+    <cfRule type="expression" dxfId="2" priority="34">
+      <formula xml:space="preserve"> $O$39&lt;&gt;$C$44</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="O18">
-    <cfRule type="expression" dxfId="21" priority="17">
-      <formula>$O$18&lt;&gt;$C$18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O32">
-    <cfRule type="expression" dxfId="20" priority="16">
-      <formula>$O$32&lt;&gt;$C$32</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O28">
-    <cfRule type="expression" dxfId="19" priority="15">
-      <formula>$O$28&lt;&gt;$C$28</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O20">
-    <cfRule type="expression" dxfId="18" priority="14">
-      <formula>$O$20&lt;&gt;$C$20</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O21">
-    <cfRule type="expression" dxfId="17" priority="13">
-      <formula>$O$21&lt;&gt;$C$21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O22">
-    <cfRule type="expression" dxfId="16" priority="12">
-      <formula>$O$22&lt;&gt;$C$22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O23">
-    <cfRule type="expression" dxfId="15" priority="11">
-      <formula>$O$23&lt;&gt;$C$23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O24">
-    <cfRule type="expression" dxfId="14" priority="10">
-      <formula>$O$24&lt;&gt;$C$24</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O25">
-    <cfRule type="expression" dxfId="13" priority="9">
-      <formula>$O$25&lt;&gt;$C$25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O26 O28">
-    <cfRule type="expression" dxfId="12" priority="8">
-      <formula>$O$26&lt;&gt;$C$26</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O27:O28">
-    <cfRule type="expression" dxfId="11" priority="7">
-      <formula>$O$27&lt;&gt;$C$27</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O29">
-    <cfRule type="expression" dxfId="10" priority="6">
-      <formula>$O$29&lt;&gt;$C$29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O30">
-    <cfRule type="expression" dxfId="9" priority="5">
-      <formula>$O$30&lt;&gt;$C$30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O31:O32">
-    <cfRule type="expression" dxfId="8" priority="4">
-      <formula>$O$31&lt;&gt;$C$31</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O34">
-    <cfRule type="expression" dxfId="7" priority="27">
-      <formula>$O$34&lt;&gt;$C$34</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O35">
-    <cfRule type="expression" dxfId="6" priority="26">
-      <formula>$O$35&lt;&gt;$C$35</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O36">
-    <cfRule type="expression" dxfId="5" priority="25">
-      <formula>$O$36&lt;&gt;$C$36</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O37">
-    <cfRule type="expression" dxfId="4" priority="24">
-      <formula>$O$37&lt;&gt;$C$37</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O39">
-    <cfRule type="expression" dxfId="3" priority="33">
-      <formula xml:space="preserve"> $O$39&lt;&gt;$C$39</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O40">
-    <cfRule type="expression" dxfId="2" priority="34">
-      <formula xml:space="preserve"> $O$40&lt;&gt;$C$45</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O19">
     <cfRule type="expression" dxfId="1" priority="48">
       <formula>#REF!&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O11">
+  <conditionalFormatting sqref="O10">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$O$11&lt;&gt;$C$11</formula>
+      <formula>$O$10&lt;&gt;$C$10</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="35" orientation="landscape" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="O11:O39 O4:O8 O9" formulaRange="1"/>
+    <ignoredError sqref="O10:O38 O4:O8" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mise à jour de la documentation de l'utilisateur
</commit_message>
<xml_diff>
--- a/docs/PlanificationV2.xlsx
+++ b/docs/PlanificationV2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\var\www\Flavio_Soares_Rodrigues_TPI_2023\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\var\www\Flavio_Soares_Rodrigues_TPI_2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBD075F-4D56-4583-B4EB-B09BE24ED301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4A0B45-FF17-485C-A2BB-3DB526005612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="33315" yWindow="7950" windowWidth="18900" windowHeight="12795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5505" yWindow="2295" windowWidth="28800" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning réel" sheetId="4" r:id="rId1"/>
@@ -739,7 +739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -887,9 +887,6 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1621,8 +1618,8 @@
   </sheetPr>
   <dimension ref="B1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="B24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -2066,7 +2063,7 @@
       <c r="O18" s="21"/>
     </row>
     <row r="19" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="7">
@@ -2093,7 +2090,7 @@
       </c>
     </row>
     <row r="20" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="50" t="s">
+      <c r="B20" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C20" s="7">
@@ -2118,7 +2115,7 @@
       </c>
     </row>
     <row r="21" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="7">
@@ -2145,7 +2142,7 @@
       </c>
     </row>
     <row r="22" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="50" t="s">
+      <c r="B22" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="7">
@@ -2170,7 +2167,7 @@
       </c>
     </row>
     <row r="23" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="50" t="s">
+      <c r="B23" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C23" s="7">
@@ -2195,7 +2192,7 @@
       </c>
     </row>
     <row r="24" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C24" s="7">
@@ -2220,7 +2217,7 @@
       </c>
     </row>
     <row r="25" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="50" t="s">
+      <c r="B25" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C25" s="7">
@@ -2245,7 +2242,7 @@
       </c>
     </row>
     <row r="26" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C26" s="7">
@@ -2269,7 +2266,7 @@
       </c>
     </row>
     <row r="27" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="50" t="s">
+      <c r="B27" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C27" s="7">
@@ -2294,7 +2291,7 @@
       </c>
     </row>
     <row r="28" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="50" t="s">
+      <c r="B28" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="7">
@@ -2319,7 +2316,7 @@
       </c>
     </row>
     <row r="29" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="50" t="s">
+      <c r="B29" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C29" s="7">
@@ -2344,7 +2341,7 @@
       </c>
     </row>
     <row r="30" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="50" t="s">
+      <c r="B30" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C30" s="7">
@@ -2369,7 +2366,7 @@
       </c>
     </row>
     <row r="31" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C31" s="7">
@@ -2445,11 +2442,13 @@
       <c r="L33" s="4">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="M33" s="4"/>
+      <c r="M33" s="4">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="N33" s="23"/>
       <c r="O33" s="9">
         <f t="shared" si="0"/>
-        <v>0.17708333333333334</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="34" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2497,11 +2496,13 @@
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
+      <c r="M35" s="4">
+        <v>0.27777777777777779</v>
+      </c>
       <c r="N35" s="23"/>
       <c r="O35" s="9">
         <f t="shared" si="0"/>
-        <v>0.38194444444444442</v>
+        <v>0.65972222222222221</v>
       </c>
     </row>
     <row r="36" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2520,11 +2521,13 @@
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
+      <c r="M36" s="4">
+        <v>4.5138888888888888E-2</v>
+      </c>
       <c r="N36" s="23"/>
       <c r="O36" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.5138888888888888E-2</v>
       </c>
     </row>
     <row r="37" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2626,7 +2629,7 @@
       </c>
       <c r="M39" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="N39" s="5">
         <f t="shared" si="3"/>
@@ -2634,7 +2637,7 @@
       </c>
       <c r="O39" s="6">
         <f>SUM(D39:N39)</f>
-        <v>3</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="P39" s="4"/>
     </row>

</xml_diff>